<commit_message>
Code updated with Page Object Model
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestDataShareSkill.xlsx
+++ b/MarsFramework/ExcelData/TestDataShareSkill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\MVPStudio-MarsProject\Internship-Mars\Assignments\Assignment-3\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D03F52E-7B31-43EB-8CD3-E42853FB4AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46819AAF-A0DB-4F33-A46A-8073C37122F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1063" yWindow="1063" windowWidth="14503" windowHeight="8931" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -22,13 +22,21 @@
     <sheet name="Skill" sheetId="7" r:id="rId7"/>
     <sheet name="Education" sheetId="8" r:id="rId8"/>
     <sheet name="Certifications" sheetId="9" r:id="rId9"/>
+    <sheet name="RequestSkillTrade" sheetId="11" r:id="rId10"/>
+    <sheet name="Chat" sheetId="12" r:id="rId11"/>
+    <sheet name="SearchSkill" sheetId="13" r:id="rId12"/>
+    <sheet name="ChangePassword" sheetId="14" r:id="rId13"/>
+    <sheet name="DescriptionProfile" sheetId="15" r:id="rId14"/>
+    <sheet name="AvailHoursEarn" sheetId="16" r:id="rId15"/>
+    <sheet name="SentRequest" sheetId="18" r:id="rId16"/>
+    <sheet name="ReceivedRequest" sheetId="19" r:id="rId17"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
   <si>
     <t>Url</t>
   </si>
@@ -192,9 +200,6 @@
     <t>Webpage Design</t>
   </si>
   <si>
-    <t>Mon</t>
-  </si>
-  <si>
     <t>8:00AM</t>
   </si>
   <si>
@@ -295,12 +300,90 @@
   </si>
   <si>
     <t>Italian</t>
+  </si>
+  <si>
+    <t>Conversational</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Message To The Seller</t>
+  </si>
+  <si>
+    <t>I am interested in your session</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Hello…..Welcome</t>
+  </si>
+  <si>
+    <t>SkillToSearch</t>
+  </si>
+  <si>
+    <t>Web Designing</t>
+  </si>
+  <si>
+    <t>Current Password</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>P@ssword1</t>
+  </si>
+  <si>
+    <t>Hi, I am Karthika. Craft making is my hobby.</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>EarnTarget</t>
+  </si>
+  <si>
+    <t>Part Time</t>
+  </si>
+  <si>
+    <t>More than 30hours a week</t>
+  </si>
+  <si>
+    <t>Between $500 and $1000 per month</t>
+  </si>
+  <si>
+    <t>SentRequest</t>
+  </si>
+  <si>
+    <t>ReceivedRequest</t>
+  </si>
+  <si>
+    <t>Category is required</t>
+  </si>
+  <si>
+    <t>22/06/2022</t>
+  </si>
+  <si>
+    <t>23/06/2022</t>
+  </si>
+  <si>
+    <t>24/06/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,13 +430,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -752,12 +837,274 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D50984-06EC-4DEB-BA4A-30C0710ED0C7}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="40.53515625" customWidth="1"/>
+    <col min="2" max="2" width="10.4609375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049D778F-FCDA-41E1-B715-28F8EA41D429}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="19.765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FA5034-CE7A-4629-AFB2-AB4CCC1D6A1B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="18.61328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22B59B7-0207-4F84-93E4-267E6F7544CC}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="19.921875" customWidth="1"/>
+    <col min="2" max="2" width="19.4609375" customWidth="1"/>
+    <col min="3" max="3" width="22.61328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0BFA19B3-0E7D-43D5-A7F5-85AC61A2ACEE}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{6C0AD62D-4A8C-4ED7-A0ED-35FBDE1F980A}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{DCA4F479-8471-4C3A-B8FA-615BE955BF12}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B88CA319-29BC-43F9-9699-689EA1601350}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="41.84375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D859429-3B87-4600-A4DE-B5321C4110EC}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="14.765625" customWidth="1"/>
+    <col min="2" max="2" width="29.07421875" customWidth="1"/>
+    <col min="3" max="3" width="40.15234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5F7AA0-4961-40E8-9E80-9D8F1E971945}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="20.23046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A3522C-7EC3-4BA6-B454-E551355E3FC4}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="20.3046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -804,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -902,11 +1249,11 @@
       <c r="G2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="3">
-        <v>44664</v>
-      </c>
-      <c r="I2" s="3">
-        <v>44664</v>
+      <c r="H2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>38</v>
@@ -955,14 +1302,14 @@
       <c r="G3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="3">
-        <v>44666</v>
-      </c>
-      <c r="I3" s="3">
-        <v>44635</v>
+      <c r="H3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="K3" t="s">
         <v>36</v>
@@ -1008,17 +1355,17 @@
       <c r="G4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="3">
-        <v>44669</v>
-      </c>
-      <c r="I4" s="3">
-        <v>44669</v>
+      <c r="H4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
         <v>54</v>
-      </c>
-      <c r="K4" t="s">
-        <v>55</v>
       </c>
       <c r="L4" t="s">
         <v>37</v>
@@ -1027,7 +1374,7 @@
         <v>14</v>
       </c>
       <c r="N4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O4" t="s">
         <v>11</v>
@@ -1041,10 +1388,13 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
         <v>57</v>
       </c>
-      <c r="B5" t="s">
-        <v>58</v>
+      <c r="C5" t="s">
+        <v>109</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1060,7 +1410,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1095,7 +1445,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1110,10 +1460,10 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -1121,7 +1471,7 @@
         <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>8</v>
@@ -1137,45 +1487,45 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="26.15234375" customWidth="1"/>
+    <col min="1" max="1" width="20.61328125" customWidth="1"/>
     <col min="2" max="2" width="23.3046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
         <v>64</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
         <v>86</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
         <v>88</v>
-      </c>
-      <c r="B4" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1199,34 +1549,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>67</v>
-      </c>
-      <c r="B2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
         <v>71</v>
-      </c>
-      <c r="B4" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1239,7 +1589,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1253,33 +1603,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
         <v>73</v>
-      </c>
-      <c r="B1" t="s">
-        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
         <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
         <v>77</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>78</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>79</v>
-      </c>
-      <c r="D2" t="s">
-        <v>80</v>
       </c>
       <c r="E2">
         <v>2010</v>
@@ -1306,21 +1656,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
         <v>81</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>82</v>
-      </c>
-      <c r="C1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
         <v>84</v>
-      </c>
-      <c r="B2" t="s">
-        <v>85</v>
       </c>
       <c r="C2">
         <v>2008</v>

</xml_diff>